<commit_message>
#10 - Modelo /risk-mc2d utiliza a biblioteca mc2d. Pode ajudar a simplificar a modelagem e após isso o tratamento dos dados.
</commit_message>
<xml_diff>
--- a/study_models/risk-pedro/Exempo_No_@Risk.xlsx
+++ b/study_models/risk-pedro/Exempo_No_@Risk.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2775" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2775" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RiskSerializationData" sheetId="9" state="hidden" r:id="rId1"/>
@@ -34259,7 +34259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O350"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P48" sqref="P48"/>
     </sheetView>
   </sheetViews>
@@ -41854,8 +41854,8 @@
   </sheetPr>
   <dimension ref="B1:K55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>